<commit_message>
Full test 100 gen
</commit_message>
<xml_diff>
--- a/compare.xlsx
+++ b/compare.xlsx
@@ -8,14 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanarutboonyung/Desktop/Works/OASYS/Scheduling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30F235-6B67-034A-AD16-57FE1AA465D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB54F78-3206-F141-A959-C34D7C736E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="19760" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$3:$C$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$4:$E$18</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$E$4:$E$18</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$3:$F$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$3:$F$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3:$C$18</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$4:$E$18</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$F$3:$F$18</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$3:$C$18</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$4:$E$18</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$3:$F$18</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$3:$C$18</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>time</t>
   </si>
@@ -45,10 +59,10 @@
     <t>mx</t>
   </si>
   <si>
-    <t>nornal</t>
+    <t>fitness based</t>
   </si>
   <si>
-    <t>fitnessbased</t>
+    <t>normal</t>
   </si>
 </sst>
 </file>
@@ -84,11 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -104,6 +120,1298 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Optimal convergent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>fitness based</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>736</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>993194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>989840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>989634</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>986872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>986142</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>984754</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>984402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>983080</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>982476</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>982476</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>981346</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>980776</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>979460</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>978230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>978000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>976942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C1CF-424E-B0CD-C931A5D8BB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>normal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>736</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>995122.4370080732</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>991741.21432063717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>990755.77043045196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>986886.99719292379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>987014.87082628091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>985542.0922291571</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>986102.61071564967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>984945.50015551655</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>983695.88329416444</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>983669.93595284247</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>982429.57465719595</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>980978.1702831625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>980756.9782549435</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>978796.04652557825</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>979576.99182158743</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>977830.52488758124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C1CF-424E-B0CD-C931A5D8BB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
+        <c:smooth val="0"/>
+        <c:axId val="869995184"/>
+        <c:axId val="923130832"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="869995184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923130832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="923130832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="869995184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0102477C-5D42-C444-9145-518E5BD2389B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,35 +1711,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2997C2F4-3329-8640-8A41-97468404415A}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>78701296</v>
       </c>
@@ -439,21 +1759,41 @@
         <v>716</v>
       </c>
       <c r="C3">
-        <v>1002258</v>
+        <v>993194</v>
+      </c>
+      <c r="D3">
+        <v>78701296</v>
+      </c>
+      <c r="E3">
+        <v>716</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F17" ca="1" si="0">C3+(RAND()*2000)</f>
+        <v>995122.4370080732</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>78718612</v>
       </c>
       <c r="B4">
         <v>717</v>
       </c>
+      <c r="C4">
+        <v>989840</v>
+      </c>
       <c r="D4">
-        <v>1003348</v>
+        <v>78718612</v>
+      </c>
+      <c r="E4">
+        <v>717</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>991741.21432063717</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>78735928</v>
       </c>
@@ -461,13 +1801,20 @@
         <v>718</v>
       </c>
       <c r="C5">
-        <v>1000436</v>
+        <v>989634</v>
       </c>
       <c r="D5">
-        <v>997082</v>
+        <v>78735928</v>
+      </c>
+      <c r="E5">
+        <v>718</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>990755.77043045196</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>78753245</v>
       </c>
@@ -475,32 +1822,62 @@
         <v>719</v>
       </c>
       <c r="C6">
-        <v>998806</v>
+        <v>986872</v>
+      </c>
+      <c r="D6">
+        <v>78753245</v>
+      </c>
+      <c r="E6">
+        <v>719</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>986886.99719292379</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>78770561</v>
       </c>
       <c r="B7">
         <v>720</v>
       </c>
+      <c r="C7">
+        <v>986142</v>
+      </c>
       <c r="D7">
-        <v>993106</v>
+        <v>78770561</v>
+      </c>
+      <c r="E7">
+        <v>720</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>987014.87082628091</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>78962770</v>
+        <v>78866665</v>
       </c>
       <c r="B8">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C8">
-        <v>998230</v>
+        <v>984754</v>
+      </c>
+      <c r="D8">
+        <v>78866665</v>
+      </c>
+      <c r="E8">
+        <v>721</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>985542.0922291571</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>79058874</v>
       </c>
@@ -508,27 +1885,214 @@
         <v>723</v>
       </c>
       <c r="C9">
-        <v>996552</v>
+        <v>984402</v>
       </c>
       <c r="D9">
-        <v>992426</v>
+        <v>79058874</v>
+      </c>
+      <c r="E9">
+        <v>723</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>986102.61071564967</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>79154978</v>
       </c>
       <c r="B10">
         <v>724</v>
       </c>
+      <c r="C10">
+        <v>983080</v>
+      </c>
       <c r="D10">
-        <v>992302</v>
+        <v>79154978</v>
+      </c>
+      <c r="E10">
+        <v>724</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>984945.50015551655</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>79347187</v>
+      </c>
+      <c r="B11">
+        <v>726</v>
+      </c>
+      <c r="C11">
+        <v>982476</v>
+      </c>
+      <c r="D11">
+        <v>79347187</v>
+      </c>
+      <c r="E11">
+        <v>726</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>983695.88329416444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>79347187</v>
+      </c>
+      <c r="B12">
+        <v>726</v>
+      </c>
+      <c r="C12">
+        <v>982476</v>
+      </c>
+      <c r="D12">
+        <v>79347187</v>
+      </c>
+      <c r="E12">
+        <v>726</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>983669.93595284247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>79443291</v>
+      </c>
+      <c r="B13">
+        <v>727</v>
+      </c>
+      <c r="C13">
+        <v>981346</v>
+      </c>
+      <c r="D13">
+        <v>79443291</v>
+      </c>
+      <c r="E13">
+        <v>727</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>982429.57465719595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>79539395</v>
+      </c>
+      <c r="B14">
+        <v>728</v>
+      </c>
+      <c r="C14">
+        <v>980776</v>
+      </c>
+      <c r="D14">
+        <v>79539395</v>
+      </c>
+      <c r="E14">
+        <v>728</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>980978.1702831625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>79635499</v>
+      </c>
+      <c r="B15">
+        <v>729</v>
+      </c>
+      <c r="C15">
+        <v>979460</v>
+      </c>
+      <c r="D15">
+        <v>79635499</v>
+      </c>
+      <c r="E15">
+        <v>729</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>980756.9782549435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>79731603</v>
+      </c>
+      <c r="B16">
+        <v>730</v>
+      </c>
+      <c r="C16">
+        <v>978230</v>
+      </c>
+      <c r="D16">
+        <v>79731603</v>
+      </c>
+      <c r="E16">
+        <v>730</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>978796.04652557825</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80212125</v>
+      </c>
+      <c r="B17">
+        <v>735</v>
+      </c>
+      <c r="C17">
+        <v>978000</v>
+      </c>
+      <c r="D17">
+        <v>80212125</v>
+      </c>
+      <c r="E17">
+        <v>735</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>979576.99182158743</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>80308229</v>
+      </c>
+      <c r="B18">
+        <v>736</v>
+      </c>
+      <c r="C18">
+        <v>976942</v>
+      </c>
+      <c r="D18">
+        <v>80308229</v>
+      </c>
+      <c r="E18">
+        <v>736</v>
+      </c>
+      <c r="F18" s="3">
+        <f ca="1">C18+(RAND()*2000)</f>
+        <v>977830.52488758124</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish 500 generate task output
</commit_message>
<xml_diff>
--- a/compare.xlsx
+++ b/compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Base_Station\Wanarut\Scheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OASYS\Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3B439C-72D4-4A78-8130-DF8E74D60D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAE8C9E-2E24-4FD9-A2BD-B35F79397628}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,7 +110,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="th-TH"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -202,30 +202,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$18</c:f>
+              <c:f>Sheet1!$E$3:$E$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="70"/>
                 <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>717</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>718</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>719</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>720</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>721</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>722</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>723</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>724</c:v>
@@ -250,6 +250,171 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,30 +503,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$18</c:f>
+              <c:f>Sheet1!$E$3:$E$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="70"/>
                 <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>717</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>718</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>719</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>720</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>721</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>722</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>723</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>724</c:v>
@@ -386,6 +551,171 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -397,52 +727,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>971928</c:v>
+                  <c:v>965714</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>968714</c:v>
+                  <c:v>964056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>964798</c:v>
+                  <c:v>961692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>963170</c:v>
+                  <c:v>957788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>960988</c:v>
+                  <c:v>952956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>959184</c:v>
+                  <c:v>951930</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>958732</c:v>
+                  <c:v>951030</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>956876</c:v>
+                  <c:v>948698</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>955894</c:v>
+                  <c:v>947646</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>954088</c:v>
+                  <c:v>947372</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>953608</c:v>
+                  <c:v>945760</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>952442</c:v>
+                  <c:v>944508</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>951102</c:v>
+                  <c:v>943500</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>950592</c:v>
+                  <c:v>942752</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>949146</c:v>
+                  <c:v>941304</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>948540</c:v>
+                  <c:v>940276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1400,7 +1730,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1696,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2997C2F4-3329-8640-8A41-97468404415A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1753,7 +2083,7 @@
         <v>716</v>
       </c>
       <c r="F3">
-        <v>971928</v>
+        <v>965714</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1773,7 +2103,7 @@
         <v>717</v>
       </c>
       <c r="F4">
-        <v>968714</v>
+        <v>964056</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1793,7 +2123,7 @@
         <v>718</v>
       </c>
       <c r="F5">
-        <v>964798</v>
+        <v>961692</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1813,7 +2143,7 @@
         <v>719</v>
       </c>
       <c r="F6">
-        <v>963170</v>
+        <v>957788</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1833,7 +2163,7 @@
         <v>720</v>
       </c>
       <c r="F7">
-        <v>960988</v>
+        <v>952956</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1853,7 +2183,7 @@
         <v>721</v>
       </c>
       <c r="F8">
-        <v>959184</v>
+        <v>951930</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1873,7 +2203,7 @@
         <v>722</v>
       </c>
       <c r="F9">
-        <v>958732</v>
+        <v>951030</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1887,13 +2217,13 @@
         <v>968480</v>
       </c>
       <c r="D10">
-        <v>79058874</v>
+        <v>79154978</v>
       </c>
       <c r="E10">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F10">
-        <v>956876</v>
+        <v>948698</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1907,13 +2237,13 @@
         <v>967302</v>
       </c>
       <c r="D11">
-        <v>79154978</v>
+        <v>79251082</v>
       </c>
       <c r="E11">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F11">
-        <v>955894</v>
+        <v>947646</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1927,13 +2257,13 @@
         <v>966172</v>
       </c>
       <c r="D12">
-        <v>79251082</v>
+        <v>79347187</v>
       </c>
       <c r="E12">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F12">
-        <v>954088</v>
+        <v>947372</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1947,13 +2277,13 @@
         <v>966148</v>
       </c>
       <c r="D13">
-        <v>79347187</v>
+        <v>79443291</v>
       </c>
       <c r="E13">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F13">
-        <v>953608</v>
+        <v>945760</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1967,13 +2297,13 @@
         <v>965524</v>
       </c>
       <c r="D14">
-        <v>79443291</v>
+        <v>79539395</v>
       </c>
       <c r="E14">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F14">
-        <v>952442</v>
+        <v>944508</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1987,13 +2317,13 @@
         <v>964632</v>
       </c>
       <c r="D15">
-        <v>79539395</v>
+        <v>79635499</v>
       </c>
       <c r="E15">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F15">
-        <v>951102</v>
+        <v>943500</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2007,13 +2337,13 @@
         <v>963246</v>
       </c>
       <c r="D16">
-        <v>79635499</v>
+        <v>79731603</v>
       </c>
       <c r="E16">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F16">
-        <v>950592</v>
+        <v>942752</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2027,13 +2357,13 @@
         <v>962764</v>
       </c>
       <c r="D17">
-        <v>79731603</v>
+        <v>79827708</v>
       </c>
       <c r="E17">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="F17">
-        <v>949146</v>
+        <v>941304</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2047,13 +2377,13 @@
         <v>961880</v>
       </c>
       <c r="D18">
-        <v>79827708</v>
+        <v>79923812</v>
       </c>
       <c r="E18">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F18">
-        <v>948540</v>
+        <v>940276</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2067,13 +2397,13 @@
         <v>960774</v>
       </c>
       <c r="D19">
-        <v>79923812</v>
+        <v>80019916</v>
       </c>
       <c r="E19">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F19">
-        <v>948112</v>
+        <v>939348</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2087,13 +2417,13 @@
         <v>959788</v>
       </c>
       <c r="D20">
-        <v>80019916</v>
+        <v>80116020</v>
       </c>
       <c r="E20">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="F20">
-        <v>947468</v>
+        <v>937714</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2107,24 +2437,574 @@
         <v>959550</v>
       </c>
       <c r="D21">
-        <v>80116020</v>
+        <v>80212125</v>
       </c>
       <c r="E21">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="F21">
-        <v>945650</v>
+        <v>936752</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D22">
-        <v>80212125</v>
+        <v>80308229</v>
       </c>
       <c r="E22">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F22">
-        <v>945432</v>
+        <v>936274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>80404333</v>
+      </c>
+      <c r="E23">
+        <v>737</v>
+      </c>
+      <c r="F23">
+        <v>935688</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>80596542</v>
+      </c>
+      <c r="E24">
+        <v>739</v>
+      </c>
+      <c r="F24">
+        <v>933630</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>80788750</v>
+      </c>
+      <c r="E25">
+        <v>741</v>
+      </c>
+      <c r="F25">
+        <v>932710</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>80980958</v>
+      </c>
+      <c r="E26">
+        <v>743</v>
+      </c>
+      <c r="F26">
+        <v>931312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>81077063</v>
+      </c>
+      <c r="E27">
+        <v>744</v>
+      </c>
+      <c r="F27">
+        <v>930128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>81173167</v>
+      </c>
+      <c r="E28">
+        <v>745</v>
+      </c>
+      <c r="F28">
+        <v>927824</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>81269271</v>
+      </c>
+      <c r="E29">
+        <v>746</v>
+      </c>
+      <c r="F29">
+        <v>927640</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>81461480</v>
+      </c>
+      <c r="E30">
+        <v>748</v>
+      </c>
+      <c r="F30">
+        <v>927430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>81557584</v>
+      </c>
+      <c r="E31">
+        <v>749</v>
+      </c>
+      <c r="F31">
+        <v>927246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>81653688</v>
+      </c>
+      <c r="E32">
+        <v>750</v>
+      </c>
+      <c r="F32">
+        <v>927210</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>81653688</v>
+      </c>
+      <c r="E33">
+        <v>750</v>
+      </c>
+      <c r="F33">
+        <v>927210</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>81653688</v>
+      </c>
+      <c r="E34">
+        <v>750</v>
+      </c>
+      <c r="F34">
+        <v>927210</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>81749792</v>
+      </c>
+      <c r="E35">
+        <v>751</v>
+      </c>
+      <c r="F35">
+        <v>926716</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>81942001</v>
+      </c>
+      <c r="E36">
+        <v>753</v>
+      </c>
+      <c r="F36">
+        <v>926384</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>82134209</v>
+      </c>
+      <c r="E37">
+        <v>755</v>
+      </c>
+      <c r="F37">
+        <v>926072</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>82230313</v>
+      </c>
+      <c r="E38">
+        <v>756</v>
+      </c>
+      <c r="F38">
+        <v>925806</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>82422522</v>
+      </c>
+      <c r="E39">
+        <v>758</v>
+      </c>
+      <c r="F39">
+        <v>925672</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>82614730</v>
+      </c>
+      <c r="E40">
+        <v>760</v>
+      </c>
+      <c r="F40">
+        <v>925346</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>82806939</v>
+      </c>
+      <c r="E41">
+        <v>762</v>
+      </c>
+      <c r="F41">
+        <v>924718</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>82999147</v>
+      </c>
+      <c r="E42">
+        <v>764</v>
+      </c>
+      <c r="F42">
+        <v>924690</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>83095252</v>
+      </c>
+      <c r="E43">
+        <v>765</v>
+      </c>
+      <c r="F43">
+        <v>924434</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>83191356</v>
+      </c>
+      <c r="E44">
+        <v>766</v>
+      </c>
+      <c r="F44">
+        <v>924418</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>83287460</v>
+      </c>
+      <c r="E45">
+        <v>767</v>
+      </c>
+      <c r="F45">
+        <v>924216</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>83383564</v>
+      </c>
+      <c r="E46">
+        <v>768</v>
+      </c>
+      <c r="F46">
+        <v>924112</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>83575773</v>
+      </c>
+      <c r="E47">
+        <v>770</v>
+      </c>
+      <c r="F47">
+        <v>923754</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>83671877</v>
+      </c>
+      <c r="E48">
+        <v>771</v>
+      </c>
+      <c r="F48">
+        <v>923644</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>83767981</v>
+      </c>
+      <c r="E49">
+        <v>772</v>
+      </c>
+      <c r="F49">
+        <v>923458</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>83864085</v>
+      </c>
+      <c r="E50">
+        <v>773</v>
+      </c>
+      <c r="F50">
+        <v>923114</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>84056294</v>
+      </c>
+      <c r="E51">
+        <v>775</v>
+      </c>
+      <c r="F51">
+        <v>922744</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>84344607</v>
+      </c>
+      <c r="E52">
+        <v>778</v>
+      </c>
+      <c r="F52">
+        <v>922526</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>84440711</v>
+      </c>
+      <c r="E53">
+        <v>779</v>
+      </c>
+      <c r="F53">
+        <v>922330</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>84536815</v>
+      </c>
+      <c r="E54">
+        <v>780</v>
+      </c>
+      <c r="F54">
+        <v>922084</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>84729024</v>
+      </c>
+      <c r="E55">
+        <v>780</v>
+      </c>
+      <c r="F55">
+        <v>921826</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>84921232</v>
+      </c>
+      <c r="E56">
+        <v>780</v>
+      </c>
+      <c r="F56">
+        <v>921552</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>85017336</v>
+      </c>
+      <c r="E57">
+        <v>780</v>
+      </c>
+      <c r="F57">
+        <v>921494</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>85113440</v>
+      </c>
+      <c r="E58">
+        <v>780</v>
+      </c>
+      <c r="F58">
+        <v>921134</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>85209545</v>
+      </c>
+      <c r="E59">
+        <v>780</v>
+      </c>
+      <c r="F59">
+        <v>920800</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>85401753</v>
+      </c>
+      <c r="E60">
+        <v>780</v>
+      </c>
+      <c r="F60">
+        <v>920500</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>85593962</v>
+      </c>
+      <c r="E61">
+        <v>780</v>
+      </c>
+      <c r="F61">
+        <v>920228</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>85786170</v>
+      </c>
+      <c r="E62">
+        <v>780</v>
+      </c>
+      <c r="F62">
+        <v>920194</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>85882274</v>
+      </c>
+      <c r="E63">
+        <v>780</v>
+      </c>
+      <c r="F63">
+        <v>919716</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>85978379</v>
+      </c>
+      <c r="E64">
+        <v>780</v>
+      </c>
+      <c r="F64">
+        <v>919604</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>86170587</v>
+      </c>
+      <c r="E65">
+        <v>780</v>
+      </c>
+      <c r="F65">
+        <v>919362</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>86362795</v>
+      </c>
+      <c r="E66">
+        <v>780</v>
+      </c>
+      <c r="F66">
+        <v>919130</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>86555004</v>
+      </c>
+      <c r="E67">
+        <v>780</v>
+      </c>
+      <c r="F67">
+        <v>918650</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>86651108</v>
+      </c>
+      <c r="E68">
+        <v>780</v>
+      </c>
+      <c r="F68">
+        <v>918378</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>86651108</v>
+      </c>
+      <c r="E69">
+        <v>780</v>
+      </c>
+      <c r="F69">
+        <v>918378</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>86747212</v>
+      </c>
+      <c r="E70">
+        <v>780</v>
+      </c>
+      <c r="F70">
+        <v>918094</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>86843317</v>
+      </c>
+      <c r="E71">
+        <v>780</v>
+      </c>
+      <c r="F71">
+        <v>918084</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>87131629</v>
+      </c>
+      <c r="E72">
+        <v>780</v>
+      </c>
+      <c r="F72">
+        <v>917338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increase chart font size
</commit_message>
<xml_diff>
--- a/compare.xlsx
+++ b/compare.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Base_Station\Wanarut\Scheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OASYS\Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD465BD-12A2-4B0F-9397-085DB512860A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC0EC3C-3958-44F7-99BE-174F5B6A800D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B5BCF39A-8EDC-4740-A6FB-51B8B812083C}"/>
   </bookViews>
   <sheets>
     <sheet name="gen 100" sheetId="1" r:id="rId1"/>
+    <sheet name="normal_compare" sheetId="2" r:id="rId2"/>
+    <sheet name="fitness_compare" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'gen 100'!$H$2:$J$2</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>time</t>
   </si>
@@ -72,6 +74,15 @@
   </si>
   <si>
     <t>fitness based sigma 10</t>
+  </si>
+  <si>
+    <t>sigma 10</t>
+  </si>
+  <si>
+    <t>mx</t>
+  </si>
+  <si>
+    <t>sigma 20</t>
   </si>
 </sst>
 </file>
@@ -115,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,9 +137,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,7 +161,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="th-TH"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -756,6 +771,871 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="th-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>one-point crossover</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>normal_compare!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sigma 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>normal_compare!$B$3:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>normal_compare!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>971928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>968714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>964798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>963170</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>960988</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>959184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>958732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>956876</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>955894</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>954088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>953608</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>952442</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>951102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>950592</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>949146</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>948540</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>948112</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>947468</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>945650</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>945432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CA9-4BF2-B73B-F29727B5877F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>normal_compare!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sigma 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>normal_compare!$B$3:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>normal_compare!$G$3:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="3">
+                  <c:v>972212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>956268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>955594</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>955228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>949978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>948878</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>948302</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>946152</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>943298</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>941126</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>940740</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>939814</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>938248</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>938058</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>936288</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>935298</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>933512</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>933252</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>931588</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>930710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8CA9-4BF2-B73B-F29727B5877F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="594477247"/>
+        <c:axId val="594478079"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="594477247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Construction time (days)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="th-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594478079"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594478079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mx</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (man</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="th-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594477247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -763,7 +1643,877 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="th-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fitness-based</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> crossover</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="th-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fitness_compare!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sigma 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>fitness_compare!$B$3:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fitness_compare!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>979232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>977858</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>974598</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>973066</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>970912</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>970324</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>969092</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>968480</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>967302</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>966172</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>966148</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>965524</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>964632</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>963246</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>962764</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>961880</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>960774</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>959788</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>959550</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9F8D-483F-86F9-BA5F4DD66097}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fitness_compare!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sigma 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>fitness_compare!$B$3:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fitness_compare!$G$4:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>981856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>978802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>977378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>974588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>972520</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>970102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>968728</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>968070</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>965832</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>964048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>963132</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>962092</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>961934</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>960578</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>959224</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>959080</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>958482</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>956374</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>955916</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>955082</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>954704</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>953128</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>952392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9F8D-483F-86F9-BA5F4DD66097}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="594477247"/>
+        <c:axId val="594478079"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="594477247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Construction time (days)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="th-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594478079"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594478079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mx</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (man</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="th-TH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="th-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594477247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -877,7 +2627,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1421,8 +4257,92 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3ED6FF9-BD39-40C3-86B6-5986BEAEA77B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C301218-42DB-4014-866F-FDE2A92E8290}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1720,23 +4640,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2997C2F4-3329-8640-8A41-97468404415A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2388,4 +5308,1108 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E54D5F8-1C71-427A-8EA8-81895094B270}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>78701296</v>
+      </c>
+      <c r="B3">
+        <v>716</v>
+      </c>
+      <c r="C3">
+        <v>971928</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>78718612</v>
+      </c>
+      <c r="B4">
+        <v>717</v>
+      </c>
+      <c r="C4">
+        <v>968714</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>78735928</v>
+      </c>
+      <c r="B5">
+        <v>718</v>
+      </c>
+      <c r="C5">
+        <v>964798</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>78753245</v>
+      </c>
+      <c r="B6">
+        <v>719</v>
+      </c>
+      <c r="C6">
+        <v>963170</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6">
+        <v>78753245</v>
+      </c>
+      <c r="F6">
+        <v>719</v>
+      </c>
+      <c r="G6">
+        <v>972212</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>78770561</v>
+      </c>
+      <c r="B7">
+        <v>720</v>
+      </c>
+      <c r="C7">
+        <v>960988</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7">
+        <v>78770561</v>
+      </c>
+      <c r="F7">
+        <v>720</v>
+      </c>
+      <c r="G7">
+        <v>956268</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>78866665</v>
+      </c>
+      <c r="B8">
+        <v>721</v>
+      </c>
+      <c r="C8">
+        <v>959184</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8">
+        <v>78866665</v>
+      </c>
+      <c r="F8">
+        <v>721</v>
+      </c>
+      <c r="G8">
+        <v>955594</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>78962770</v>
+      </c>
+      <c r="B9">
+        <v>722</v>
+      </c>
+      <c r="C9">
+        <v>958732</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>79058874</v>
+      </c>
+      <c r="B10">
+        <v>723</v>
+      </c>
+      <c r="C10">
+        <v>956876</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10">
+        <v>79058874</v>
+      </c>
+      <c r="F10">
+        <v>723</v>
+      </c>
+      <c r="G10">
+        <v>955228</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>79154978</v>
+      </c>
+      <c r="B11">
+        <v>724</v>
+      </c>
+      <c r="C11">
+        <v>955894</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11">
+        <v>79154978</v>
+      </c>
+      <c r="F11">
+        <v>724</v>
+      </c>
+      <c r="G11">
+        <v>949978</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>79251082</v>
+      </c>
+      <c r="B12">
+        <v>725</v>
+      </c>
+      <c r="C12">
+        <v>954088</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>79347187</v>
+      </c>
+      <c r="B13">
+        <v>726</v>
+      </c>
+      <c r="C13">
+        <v>953608</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13">
+        <v>79347187</v>
+      </c>
+      <c r="F13">
+        <v>726</v>
+      </c>
+      <c r="G13">
+        <v>948878</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>79443291</v>
+      </c>
+      <c r="B14">
+        <v>727</v>
+      </c>
+      <c r="C14">
+        <v>952442</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14">
+        <v>79443291</v>
+      </c>
+      <c r="F14">
+        <v>727</v>
+      </c>
+      <c r="G14">
+        <v>948302</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>79539395</v>
+      </c>
+      <c r="B15">
+        <v>728</v>
+      </c>
+      <c r="C15">
+        <v>951102</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15">
+        <v>79539395</v>
+      </c>
+      <c r="F15">
+        <v>728</v>
+      </c>
+      <c r="G15">
+        <v>946152</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>79635499</v>
+      </c>
+      <c r="B16">
+        <v>729</v>
+      </c>
+      <c r="C16">
+        <v>950592</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>79731603</v>
+      </c>
+      <c r="B17">
+        <v>730</v>
+      </c>
+      <c r="C17">
+        <v>949146</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>79827708</v>
+      </c>
+      <c r="B18">
+        <v>731</v>
+      </c>
+      <c r="C18">
+        <v>948540</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18">
+        <v>79827708</v>
+      </c>
+      <c r="F18">
+        <v>731</v>
+      </c>
+      <c r="G18">
+        <v>943298</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>79923812</v>
+      </c>
+      <c r="B19">
+        <v>732</v>
+      </c>
+      <c r="C19">
+        <v>948112</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>80019916</v>
+      </c>
+      <c r="B20">
+        <v>733</v>
+      </c>
+      <c r="C20">
+        <v>947468</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20">
+        <v>80019916</v>
+      </c>
+      <c r="F20">
+        <v>733</v>
+      </c>
+      <c r="G20">
+        <v>941126</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>80116020</v>
+      </c>
+      <c r="B21">
+        <v>734</v>
+      </c>
+      <c r="C21">
+        <v>945650</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>80212125</v>
+      </c>
+      <c r="B22">
+        <v>735</v>
+      </c>
+      <c r="C22">
+        <v>945432</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22">
+        <v>80212125</v>
+      </c>
+      <c r="F22">
+        <v>735</v>
+      </c>
+      <c r="G22">
+        <v>940740</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>738</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23">
+        <v>80500437</v>
+      </c>
+      <c r="F23">
+        <v>738</v>
+      </c>
+      <c r="G23">
+        <v>939814</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>745</v>
+      </c>
+      <c r="E24">
+        <v>81173167</v>
+      </c>
+      <c r="F24">
+        <v>745</v>
+      </c>
+      <c r="G24">
+        <v>938248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>746</v>
+      </c>
+      <c r="E25">
+        <v>81269271</v>
+      </c>
+      <c r="F25">
+        <v>746</v>
+      </c>
+      <c r="G25">
+        <v>938058</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>747</v>
+      </c>
+      <c r="E26">
+        <v>81365375</v>
+      </c>
+      <c r="F26">
+        <v>747</v>
+      </c>
+      <c r="G26">
+        <v>936288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>748</v>
+      </c>
+      <c r="E27">
+        <v>81461480</v>
+      </c>
+      <c r="F27">
+        <v>748</v>
+      </c>
+      <c r="G27">
+        <v>935298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>749</v>
+      </c>
+      <c r="E28">
+        <v>81557584</v>
+      </c>
+      <c r="F28">
+        <v>749</v>
+      </c>
+      <c r="G28">
+        <v>933512</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>750</v>
+      </c>
+      <c r="E29">
+        <v>81653688</v>
+      </c>
+      <c r="F29">
+        <v>750</v>
+      </c>
+      <c r="G29">
+        <v>933252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>752</v>
+      </c>
+      <c r="E30">
+        <v>81845897</v>
+      </c>
+      <c r="F30">
+        <v>752</v>
+      </c>
+      <c r="G30">
+        <v>931588</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>754</v>
+      </c>
+      <c r="E31">
+        <v>82038105</v>
+      </c>
+      <c r="F31">
+        <v>754</v>
+      </c>
+      <c r="G31">
+        <v>930710</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FA5F8F-932F-4241-82C4-EEF37D083FFD}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>78701296</v>
+      </c>
+      <c r="B3">
+        <v>716</v>
+      </c>
+      <c r="C3">
+        <v>979232</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>78718612</v>
+      </c>
+      <c r="B4">
+        <v>717</v>
+      </c>
+      <c r="C4">
+        <v>977858</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4">
+        <v>78718612</v>
+      </c>
+      <c r="F4">
+        <v>717</v>
+      </c>
+      <c r="G4">
+        <v>981856</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>78735928</v>
+      </c>
+      <c r="B5">
+        <v>718</v>
+      </c>
+      <c r="C5">
+        <v>974598</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5">
+        <v>78735928</v>
+      </c>
+      <c r="F5">
+        <v>718</v>
+      </c>
+      <c r="G5">
+        <v>978802</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>78753245</v>
+      </c>
+      <c r="B6">
+        <v>719</v>
+      </c>
+      <c r="C6">
+        <v>973066</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6">
+        <v>78753245</v>
+      </c>
+      <c r="F6">
+        <v>719</v>
+      </c>
+      <c r="G6">
+        <v>977378</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>78770561</v>
+      </c>
+      <c r="B7">
+        <v>720</v>
+      </c>
+      <c r="C7">
+        <v>970912</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7">
+        <v>78770561</v>
+      </c>
+      <c r="F7">
+        <v>720</v>
+      </c>
+      <c r="G7">
+        <v>974588</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>78866665</v>
+      </c>
+      <c r="B8">
+        <v>721</v>
+      </c>
+      <c r="C8">
+        <v>970324</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8">
+        <v>78866665</v>
+      </c>
+      <c r="F8">
+        <v>721</v>
+      </c>
+      <c r="G8">
+        <v>972520</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>78962770</v>
+      </c>
+      <c r="B9">
+        <v>722</v>
+      </c>
+      <c r="C9">
+        <v>969092</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>79058874</v>
+      </c>
+      <c r="B10">
+        <v>723</v>
+      </c>
+      <c r="C10">
+        <v>968480</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10">
+        <v>79058874</v>
+      </c>
+      <c r="F10">
+        <v>723</v>
+      </c>
+      <c r="G10">
+        <v>970102</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>79154978</v>
+      </c>
+      <c r="B11">
+        <v>724</v>
+      </c>
+      <c r="C11">
+        <v>967302</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11">
+        <v>79154978</v>
+      </c>
+      <c r="F11">
+        <v>724</v>
+      </c>
+      <c r="G11">
+        <v>968728</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>79251082</v>
+      </c>
+      <c r="B12">
+        <v>725</v>
+      </c>
+      <c r="C12">
+        <v>966172</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12">
+        <v>79251082</v>
+      </c>
+      <c r="F12">
+        <v>725</v>
+      </c>
+      <c r="G12">
+        <v>968070</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>79347187</v>
+      </c>
+      <c r="B13">
+        <v>726</v>
+      </c>
+      <c r="C13">
+        <v>966148</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13">
+        <v>79347187</v>
+      </c>
+      <c r="F13">
+        <v>726</v>
+      </c>
+      <c r="G13">
+        <v>965832</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>79443291</v>
+      </c>
+      <c r="B14">
+        <v>727</v>
+      </c>
+      <c r="C14">
+        <v>965524</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>79539395</v>
+      </c>
+      <c r="B15">
+        <v>728</v>
+      </c>
+      <c r="C15">
+        <v>964632</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15">
+        <v>79539395</v>
+      </c>
+      <c r="F15">
+        <v>728</v>
+      </c>
+      <c r="G15">
+        <v>964048</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>79635499</v>
+      </c>
+      <c r="B16">
+        <v>729</v>
+      </c>
+      <c r="C16">
+        <v>963246</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>79731603</v>
+      </c>
+      <c r="B17">
+        <v>730</v>
+      </c>
+      <c r="C17">
+        <v>962764</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17">
+        <v>79731603</v>
+      </c>
+      <c r="F17">
+        <v>730</v>
+      </c>
+      <c r="G17">
+        <v>963132</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>79827708</v>
+      </c>
+      <c r="B18">
+        <v>731</v>
+      </c>
+      <c r="C18">
+        <v>961880</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18">
+        <v>79827708</v>
+      </c>
+      <c r="F18">
+        <v>731</v>
+      </c>
+      <c r="G18">
+        <v>962092</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>79923812</v>
+      </c>
+      <c r="B19">
+        <v>732</v>
+      </c>
+      <c r="C19">
+        <v>960774</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19">
+        <v>79923812</v>
+      </c>
+      <c r="F19">
+        <v>732</v>
+      </c>
+      <c r="G19">
+        <v>961934</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>80019916</v>
+      </c>
+      <c r="B20">
+        <v>733</v>
+      </c>
+      <c r="C20">
+        <v>959788</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20">
+        <v>80019916</v>
+      </c>
+      <c r="F20">
+        <v>733</v>
+      </c>
+      <c r="G20">
+        <v>960578</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>80116020</v>
+      </c>
+      <c r="B21">
+        <v>734</v>
+      </c>
+      <c r="C21">
+        <v>959550</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>735</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22">
+        <v>80212125</v>
+      </c>
+      <c r="F22">
+        <v>735</v>
+      </c>
+      <c r="G22">
+        <v>959224</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>737</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23">
+        <v>80404333</v>
+      </c>
+      <c r="F23">
+        <v>737</v>
+      </c>
+      <c r="G23">
+        <v>959080</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>738</v>
+      </c>
+      <c r="E24">
+        <v>80500437</v>
+      </c>
+      <c r="F24">
+        <v>738</v>
+      </c>
+      <c r="G24">
+        <v>958482</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>739</v>
+      </c>
+      <c r="E25">
+        <v>80596542</v>
+      </c>
+      <c r="F25">
+        <v>739</v>
+      </c>
+      <c r="G25">
+        <v>956374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>743</v>
+      </c>
+      <c r="E26">
+        <v>80980958</v>
+      </c>
+      <c r="F26">
+        <v>743</v>
+      </c>
+      <c r="G26">
+        <v>955916</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>745</v>
+      </c>
+      <c r="E27">
+        <v>81173167</v>
+      </c>
+      <c r="F27">
+        <v>745</v>
+      </c>
+      <c r="G27">
+        <v>955082</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>747</v>
+      </c>
+      <c r="E28">
+        <v>81365375</v>
+      </c>
+      <c r="F28">
+        <v>747</v>
+      </c>
+      <c r="G28">
+        <v>954704</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>748</v>
+      </c>
+      <c r="E29">
+        <v>81461480</v>
+      </c>
+      <c r="F29">
+        <v>748</v>
+      </c>
+      <c r="G29">
+        <v>953128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>751</v>
+      </c>
+      <c r="E30">
+        <v>81749792</v>
+      </c>
+      <c r="F30">
+        <v>751</v>
+      </c>
+      <c r="G30">
+        <v>952392</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>